<commit_message>
Update excel upload, import and download
</commit_message>
<xml_diff>
--- a/excelPath/test/testChartModule2ExcelRead.xlsx
+++ b/excelPath/test/testChartModule2ExcelRead.xlsx
@@ -1,45 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\nodejs\EagleEye-Platform\excelPath\test\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18192" windowHeight="8508"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505"/>
   </bookViews>
   <sheets>
-    <sheet name="Data" sheetId="1" r:id="rId1"/>
+    <sheet name="Data" sheetId="1" r:id="rId4"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
-    <t>Category</t>
+    <t>Name</t>
   </si>
   <si>
-    <t>value1</t>
+    <t>Id</t>
   </si>
   <si>
-    <t>value2</t>
+    <t>TestFile</t>
   </si>
   <si>
-    <t>Apple</t>
+    <t>John Doe</t>
   </si>
   <si>
-    <t>Orange</t>
-  </si>
-  <si>
-    <t>value3</t>
-  </si>
-  <si>
-    <t>Banana</t>
+    <t>Jane Doe</t>
   </si>
 </sst>
 </file>
@@ -48,11 +37,11 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
-      <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+      <sz val="11"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="2">
@@ -86,9 +75,6 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -137,7 +123,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -172,7 +158,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -239,20 +225,16 @@
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:shade val="51000"/>
+                <a:tint val="100000"/>
+                <a:shade val="100000"/>
                 <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="80000">
-              <a:schemeClr val="phClr">
-                <a:shade val="93000"/>
-                <a:satMod val="130000"/>
-              </a:schemeClr>
-            </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:shade val="94000"/>
-                <a:satMod val="135000"/>
+                <a:tint val="50000"/>
+                <a:shade val="100000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
@@ -374,7 +356,46 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
-  <a:objectDefaults/>
+  <a:objectDefaults>
+    <a:spDef>
+      <a:spPr/>
+      <a:bodyPr/>
+      <a:lstStyle/>
+      <a:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="3">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </a:style>
+    </a:spDef>
+    <a:lnDef>
+      <a:spPr/>
+      <a:bodyPr/>
+      <a:lstStyle/>
+      <a:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </a:style>
+    </a:lnDef>
+  </a:objectDefaults>
   <a:extraClrSchemeLst/>
 </a:theme>
 </file>
@@ -382,17 +403,20 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
-    <tabColor rgb="FFFC0000"/>
+    <tabColor rgb="FFC0000"/>
   </sheetPr>
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="32" customWidth="1"/>
+    <col min="2" max="2" width="10" customWidth="1"/>
+    <col min="3" max="3" width="20" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -402,50 +426,27 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
-        <v>5</v>
-      </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
       <c r="B2">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C2">
-        <v>9</v>
-      </c>
-      <c r="D2">
-        <v>11</v>
+        <v>123</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
       <c r="B3">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="C3">
-        <v>3</v>
-      </c>
-      <c r="D3">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4">
-        <v>9</v>
-      </c>
-      <c r="C4">
-        <v>5</v>
-      </c>
-      <c r="D4">
-        <v>14</v>
+        <v>456</v>
       </c>
     </row>
   </sheetData>

</xml_diff>